<commit_message>
error in excel file
</commit_message>
<xml_diff>
--- a/data-output/res_ext.xlsx
+++ b/data-output/res_ext.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misst\OneDrive\Desktop\New folder\edge_detection_operators_lqimages\data-output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC8409B4-F08F-4D01-9EFA-DD217A578A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F34AB-DD7D-4526-A4DD-7E46477172EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{866DF791-9222-40A2-A28C-6160BC8A57C4}"/>
   </bookViews>
@@ -94,8 +94,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="0.000000"/>
-    <numFmt numFmtId="176" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,39 +128,39 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.0000000000"/>
+      <numFmt numFmtId="165" formatCode="0.0000000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.0000000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="0.0000000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,8 +186,8 @@
     <tableColumn id="5" xr3:uid="{67E27A1B-C80D-442E-BC2D-0945CA9456D7}" name="Sobel" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{BA32BCEB-40AF-420E-A289-6AA57E3B67CD}" name="Scharr" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{5CD94E9B-A64D-419F-9EF2-70117CA786B8}" name="Roberta" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{BD9F011C-CE19-4DD1-9C6A-E499F0A39BA8}" name="FIT" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{D69CF2EC-7889-4DCC-9A6F-9397D4C78415}" name="MAX" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{BD9F011C-CE19-4DD1-9C6A-E499F0A39BA8}" name="FIT" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{D69CF2EC-7889-4DCC-9A6F-9397D4C78415}" name="MAX" dataDxfId="1">
       <calculatedColumnFormula>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{0E583406-B71F-4685-A945-2AAC69987A7B}" name="MIN" dataDxfId="0">
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C5AADE-F371-4A77-AED1-2C2CE4126851}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,7 +566,7 @@
         <v>1.7578348085214201E-2</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
         <v>Sobel</v>
       </c>
       <c r="J2" s="2" t="str">
@@ -600,8 +600,8 @@
         <v>0.37871449459723</v>
       </c>
       <c r="I3" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
-        <v>FIT</v>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
+        <v>Scharr</v>
       </c>
       <c r="J3" s="2" t="str">
         <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MIN(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
@@ -634,8 +634,8 @@
         <v>0.17437916746370999</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
-        <v>FIT</v>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
+        <v>Scharr</v>
       </c>
       <c r="J4" s="2" t="str">
         <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MIN(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
@@ -668,7 +668,7 @@
         <v>0.142450056330202</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
         <v>Sobel</v>
       </c>
       <c r="J5" s="2" t="str">
@@ -702,8 +702,8 @@
         <v>4.6634330538651902E-2</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
-        <v>FIT</v>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
+        <v>Scharr</v>
       </c>
       <c r="J6" s="2" t="str">
         <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MIN(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
@@ -736,8 +736,8 @@
         <v>8.3220152971310093E-2</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
-        <v>FIT</v>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
+        <v>Scharr</v>
       </c>
       <c r="J7" s="2" t="str">
         <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MIN(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
@@ -770,8 +770,8 @@
         <v>9.3602211680352099E-2</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]]))</f>
-        <v>FIT</v>
+        <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MAX(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
+        <v>Scharr</v>
       </c>
       <c r="J8" s="2" t="str">
         <f>INDEX(Table1[[#Headers],[Laplasa]:[FIT]], MATCH(MIN(Table1[[#This Row],[Laplasa]:[FIT]]), Table1[[#This Row],[Laplasa]:[FIT]], 0))</f>
@@ -783,32 +783,32 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="str">
-        <f>INDEX($A$2:$A$8, MATCH(MAX(B2:B8), B2:B8))</f>
-        <v>k-izplūdis-h</v>
+        <f>INDEX($A$2:$A$8, MATCH(MAX(B2:B8), B2:B8, 0))</f>
+        <v>izklīsts</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f>INDEX($A$2:$A$8, MATCH(MAX(C2:C8), C2:C8))</f>
-        <v>k-izplūdis-h</v>
+        <f t="shared" ref="C9:H9" si="0">INDEX($A$2:$A$8, MATCH(MAX(C2:C8), C2:C8, 0))</f>
+        <v>izklīsts</v>
       </c>
       <c r="D9" s="1" t="str">
-        <f t="shared" ref="D9:H9" si="0">INDEX($A$2:$A$8, MATCH(MAX(D2:D8), D2:D8))</f>
-        <v>k-izplūdis-h</v>
+        <f t="shared" si="0"/>
+        <v>gamma-t</v>
       </c>
       <c r="E9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>k-izplūdis-h</v>
+        <v>izklīsts</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>k-izplūdis-h</v>
+        <v>izklīsts</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>k-izplūdis-h</v>
+        <v>gamma-t</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>k-izplūdis-h</v>
+        <v>izklīsts</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>

</xml_diff>